<commit_message>
Final adaptations of code
</commit_message>
<xml_diff>
--- a/output/final-figures/baltab_auctions.xlsx
+++ b/output/final-figures/baltab_auctions.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
@@ -13,95 +13,53 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="124" uniqueCount="80">
   <si>
     <t/>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Variable</t>
   </si>
   <si>
     <t>number of bidders</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>total MW auctioned</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>international bidders invited</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>projects in solar park</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>location in India</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>climate zone of plant location</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>technology neutral</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>ground-mounted, rooftop or floating plant</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>max. plant size</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>final bid price, INR/kwh</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>length of contract</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>international quality standards</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>viability-gap-funding, INR</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -162,9 +120,6 @@
     <t>1.00</t>
   </si>
   <si>
-    <t>[0.00]</t>
-  </si>
-  <si>
     <t>183.31</t>
   </si>
   <si>
@@ -180,15 +135,9 @@
     <t>25.00</t>
   </si>
   <si>
-    <t>[0.00]</t>
-  </si>
-  <si>
     <t>11.88</t>
   </si>
   <si>
-    <t>[0.50]</t>
-  </si>
-  <si>
     <t>43275870.30</t>
   </si>
   <si>
@@ -198,18 +147,12 @@
     <t>16</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>(2)</t>
   </si>
   <si>
     <t>LCR auction</t>
   </si>
   <si>
-    <t>Mean/SD</t>
-  </si>
-  <si>
     <t>5.71</t>
   </si>
   <si>
@@ -231,9 +174,6 @@
     <t>0.14</t>
   </si>
   <si>
-    <t>[0.38]</t>
-  </si>
-  <si>
     <t>6.43</t>
   </si>
   <si>
@@ -246,18 +186,6 @@
     <t>[0.69]</t>
   </si>
   <si>
-    <t>2.00</t>
-  </si>
-  <si>
-    <t>[0.00]</t>
-  </si>
-  <si>
-    <t>1.00</t>
-  </si>
-  <si>
-    <t>[0.00]</t>
-  </si>
-  <si>
     <t>26.71</t>
   </si>
   <si>
@@ -270,12 +198,6 @@
     <t>[0.54]</t>
   </si>
   <si>
-    <t>25.00</t>
-  </si>
-  <si>
-    <t>[0.00]</t>
-  </si>
-  <si>
     <t>11.43</t>
   </si>
   <si>
@@ -291,9 +213,6 @@
     <t>7</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>t-test</t>
   </si>
   <si>
@@ -306,91 +225,40 @@
     <t>0.12</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>0.01***</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>0.60</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>0.23</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>0.58</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>0.42</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>0.02**</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>0.00***</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>0.25</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>0.47</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -427,8 +295,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -436,433 +307,433 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>101</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="D11" t="s">
-        <v>103</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="s">
         <v>73</v>
-      </c>
-      <c r="D12" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s">
-        <v>105</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
-        <v>107</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>109</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>111</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="D20" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s">
-        <v>113</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>114</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="D23" t="s">
-        <v>115</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>85</v>
+        <v>39</v>
       </c>
       <c r="D24" t="s">
-        <v>116</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>86</v>
+        <v>33</v>
       </c>
       <c r="D25" t="s">
-        <v>117</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="D26" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="D27" t="s">
-        <v>119</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="D28" t="s">
-        <v>120</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="D29" t="s">
-        <v>121</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="D30" t="s">
-        <v>122</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>123</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>